<commit_message>
Adeguamenti checklist per i casi d'uso KO (precisato il worckflow) come richiesto nella mail del 17/05
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
+++ b/GATEWAY/A1#111CONSORZIOMETIS/CONSORZIO_METIS/SISPC/V.23/accreditamento-checklist.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="259">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -493,7 +493,7 @@
     <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">I dati che alimentano questo cda.xml vengono inseriti in un elenco che le utenze specifiche individuate come i referenti aziendali possono verificare e correggere</t>
+    <t xml:space="preserve">Gli errori di tipo semantico e/o terminologico vengono evidenziati agli amministratori di sistema che provvedono alla correzione/inserimento delle codifiche, alla bonifica del dato e il sistema provvede al reinvio automatico al FSE  dei documenti a queste collegati </t>
   </si>
   <si>
     <t xml:space="preserve">KO</t>
@@ -589,7 +589,7 @@
 Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nella colonna "J" nominata come "GESTIONE ERRORE".</t>
   </si>
   <si>
-    <t xml:space="preserve">Procediamo con nuovi tentativi dilazionati nel tempo</t>
+    <t xml:space="preserve">Procediamo con nuovi tentativi effettuati tramite una coda che provvede automaticamente a trasmettere nuovamente in modo dilazionato nel tempo</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_SING_VAC_TIMEOUT</t>
@@ -603,6 +603,9 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
+    <t xml:space="preserve">inseriamo sempre Normal</t>
+  </si>
+  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_CERT_VAC_CT6_KO</t>
   </si>
   <si>
@@ -621,9 +624,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">inseriamo sempre Normal</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_CERT_VAC_CT8_KO</t>
   </si>
   <si>
@@ -632,7 +632,7 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test CERT_VACC" e "CDA2_Certificato Vaccinale_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">Il comune è un campo obbligstorio dell'indirizzo di residenza</t>
+    <t xml:space="preserve">Il comune è un campo obbligatorio dell'indirizzo di residenza</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_CERT_VAC_CT9_KO</t>
@@ -752,15 +752,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test SING_VACC" e "CDA2_Scheda_Singola Vaccinazione_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-03T15:50:39Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1b1e43ef112d6b75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.90.4.4.41309ad9ee4a4dc5d8d043451d8fd76972699d3f573504fe5a355b3cfe1feb28.91a491e549^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_SING_VAC_CT6_KO</t>
   </si>
   <si>
@@ -785,6 +776,9 @@
   <si>
     <t xml:space="preserve">Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test SING_VACC" e "CDA2_Scheda_Singola Vaccinazione_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il comune è un campo obbligstorio dell'indirizzo di residenza</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_SING_VAC_CT9_KO</t>
@@ -1302,7 +1296,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1435,7 +1429,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1456,10 +1450,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1469,6 +1459,14 @@
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1621,8 +1619,8 @@
   </sheetPr>
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="F10:I10 A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2695,8 +2693,8 @@
   </sheetPr>
   <dimension ref="A1:B998"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F10:I10 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3800,12 +3798,12 @@
   </sheetPr>
   <dimension ref="A1:T669"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="K49" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I10" activeCellId="0" sqref="F10:I10"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="P51" activeCellId="0" sqref="P51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3819,7 +3817,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="27.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="11" style="2" width="36.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="27.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="38.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="33.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="2" width="36.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="2" width="31.86"/>
@@ -4105,13 +4103,13 @@
       <c r="F11" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="38" t="s">
+      <c r="H11" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="38" t="s">
+      <c r="I11" s="33" t="s">
         <v>60</v>
       </c>
       <c r="J11" s="34" t="s">
@@ -4149,13 +4147,13 @@
       <c r="F12" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="33" t="s">
         <v>65</v>
       </c>
       <c r="J12" s="34" t="s">
@@ -4193,13 +4191,13 @@
       <c r="F13" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="38" t="s">
+      <c r="H13" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="38" t="s">
+      <c r="I13" s="33" t="s">
         <v>70</v>
       </c>
       <c r="J13" s="34" t="s">
@@ -4237,13 +4235,13 @@
       <c r="F14" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="33" t="s">
         <v>76</v>
       </c>
       <c r="J14" s="34" t="s">
@@ -4281,13 +4279,13 @@
       <c r="F15" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H15" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="I15" s="38" t="s">
+      <c r="I15" s="33" t="s">
         <v>81</v>
       </c>
       <c r="J15" s="34" t="s">
@@ -4325,13 +4323,13 @@
       <c r="F16" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G16" s="39" t="s">
+      <c r="G16" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="H16" s="39" t="s">
+      <c r="H16" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="I16" s="39" t="s">
+      <c r="I16" s="38" t="s">
         <v>86</v>
       </c>
       <c r="J16" s="34" t="s">
@@ -4369,13 +4367,13 @@
       <c r="F17" s="32" t="n">
         <v>45056</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="H17" s="39" t="s">
+      <c r="H17" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="38" t="s">
         <v>91</v>
       </c>
       <c r="J17" s="34" t="s">
@@ -4394,7 +4392,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="n">
         <v>33</v>
       </c>
@@ -4407,19 +4405,19 @@
       <c r="D18" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="41" t="n">
+      <c r="F18" s="40" t="n">
         <v>44964</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="41" t="s">
+      <c r="H18" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="I18" s="41" t="s">
+      <c r="I18" s="40" t="s">
         <v>96</v>
       </c>
       <c r="J18" s="34" t="s">
@@ -4436,7 +4434,7 @@
       <c r="O18" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P18" s="34" t="s">
+      <c r="P18" s="41" t="s">
         <v>98</v>
       </c>
       <c r="Q18" s="34"/>
@@ -4446,7 +4444,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="114.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="135.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="n">
         <v>34</v>
       </c>
@@ -4459,7 +4457,7 @@
       <c r="D19" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="39" t="s">
         <v>93</v>
       </c>
       <c r="F19" s="32" t="n">
@@ -4488,7 +4486,7 @@
       <c r="O19" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P19" s="34" t="s">
+      <c r="P19" s="42" t="s">
         <v>98</v>
       </c>
       <c r="Q19" s="34"/>
@@ -4498,7 +4496,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="111.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="29" t="n">
         <v>41</v>
       </c>
@@ -4511,19 +4509,19 @@
       <c r="D20" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="40" t="s">
+      <c r="E20" s="39" t="s">
         <v>105</v>
       </c>
       <c r="F20" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="H20" s="42" t="s">
+      <c r="H20" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="I20" s="42" t="s">
+      <c r="I20" s="43" t="s">
         <v>108</v>
       </c>
       <c r="J20" s="34" t="s">
@@ -4540,7 +4538,7 @@
       <c r="O20" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P20" s="34" t="s">
+      <c r="P20" s="42" t="s">
         <v>98</v>
       </c>
       <c r="Q20" s="34"/>
@@ -4563,7 +4561,7 @@
       <c r="D21" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="39" t="s">
         <v>105</v>
       </c>
       <c r="F21" s="32" t="n">
@@ -4592,7 +4590,7 @@
       <c r="O21" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P21" s="34" t="s">
+      <c r="P21" s="42" t="s">
         <v>98</v>
       </c>
       <c r="Q21" s="34"/>
@@ -4602,7 +4600,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="29" t="n">
         <v>49</v>
       </c>
@@ -4619,9 +4617,9 @@
         <v>113</v>
       </c>
       <c r="F22" s="32"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
       <c r="J22" s="34" t="s">
         <v>54</v>
       </c>
@@ -4642,7 +4640,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="80.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="n">
         <v>50</v>
       </c>
@@ -4659,9 +4657,9 @@
         <v>113</v>
       </c>
       <c r="F23" s="32"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
       <c r="J23" s="34" t="s">
         <v>54</v>
       </c>
@@ -4682,7 +4680,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="102.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="29" t="n">
         <v>94</v>
       </c>
@@ -4698,35 +4696,21 @@
       <c r="E24" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="F24" s="32" t="n">
-        <v>44964</v>
-      </c>
-      <c r="G24" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="H24" s="42" t="s">
-        <v>95</v>
-      </c>
-      <c r="I24" s="42" t="s">
-        <v>96</v>
-      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
       <c r="J24" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="M24" s="34" t="s">
         <v>97</v>
       </c>
+      <c r="K24" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
       <c r="N24" s="34"/>
-      <c r="O24" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="P24" s="34" t="s">
-        <v>98</v>
-      </c>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
       <c r="Q24" s="34"/>
       <c r="R24" s="35"/>
       <c r="S24" s="36"/>
@@ -4745,20 +4729,20 @@
         <v>48</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F25" s="32"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
       <c r="J25" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="L25" s="34"/>
       <c r="M25" s="34"/>
@@ -4783,20 +4767,20 @@
         <v>48</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F26" s="32"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
       <c r="J26" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K26" s="34" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="L26" s="34"/>
       <c r="M26" s="34"/>
@@ -4810,7 +4794,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="29" t="n">
         <v>97</v>
       </c>
@@ -4827,9 +4811,9 @@
         <v>125</v>
       </c>
       <c r="F27" s="32"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
       <c r="J27" s="34" t="s">
         <v>97</v>
       </c>
@@ -4865,9 +4849,9 @@
         <v>128</v>
       </c>
       <c r="F28" s="32"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
       <c r="J28" s="34" t="s">
         <v>97</v>
       </c>
@@ -4903,9 +4887,9 @@
         <v>131</v>
       </c>
       <c r="F29" s="32"/>
-      <c r="G29" s="42"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
       <c r="J29" s="34" t="s">
         <v>97</v>
       </c>
@@ -4941,9 +4925,9 @@
         <v>134</v>
       </c>
       <c r="F30" s="32"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
       <c r="J30" s="34" t="s">
         <v>97</v>
       </c>
@@ -4979,9 +4963,9 @@
         <v>137</v>
       </c>
       <c r="F31" s="32"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
       <c r="J31" s="34" t="s">
         <v>97</v>
       </c>
@@ -5000,7 +4984,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="96.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="n">
         <v>102</v>
       </c>
@@ -5019,13 +5003,13 @@
       <c r="F32" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G32" s="42" t="s">
+      <c r="G32" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="H32" s="42" t="s">
+      <c r="H32" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="I32" s="42" t="s">
+      <c r="I32" s="43" t="s">
         <v>143</v>
       </c>
       <c r="J32" s="34" t="s">
@@ -5042,7 +5026,7 @@
       <c r="O32" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P32" s="34" t="s">
+      <c r="P32" s="42" t="s">
         <v>98</v>
       </c>
       <c r="Q32" s="34"/>
@@ -5052,7 +5036,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="29" t="n">
         <v>103</v>
       </c>
@@ -5071,13 +5055,13 @@
       <c r="F33" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G33" s="42" t="s">
+      <c r="G33" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="H33" s="42" t="s">
+      <c r="H33" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="I33" s="42" t="s">
+      <c r="I33" s="43" t="s">
         <v>148</v>
       </c>
       <c r="J33" s="34" t="s">
@@ -5094,7 +5078,7 @@
       <c r="O33" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P33" s="34" t="s">
+      <c r="P33" s="42" t="s">
         <v>98</v>
       </c>
       <c r="Q33" s="34"/>
@@ -5104,7 +5088,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="78.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="105.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="29" t="n">
         <v>104</v>
       </c>
@@ -5123,13 +5107,13 @@
       <c r="F34" s="32" t="n">
         <v>44964</v>
       </c>
-      <c r="G34" s="42" t="s">
+      <c r="G34" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="H34" s="42" t="s">
+      <c r="H34" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="I34" s="42" t="s">
+      <c r="I34" s="43" t="s">
         <v>153</v>
       </c>
       <c r="J34" s="34" t="s">
@@ -5146,7 +5130,7 @@
       <c r="O34" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P34" s="34" t="s">
+      <c r="P34" s="42" t="s">
         <v>98</v>
       </c>
       <c r="Q34" s="34"/>
@@ -5173,9 +5157,9 @@
         <v>155</v>
       </c>
       <c r="F35" s="32"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
       <c r="J35" s="34" t="s">
         <v>97</v>
       </c>
@@ -5211,9 +5195,9 @@
         <v>157</v>
       </c>
       <c r="F36" s="32"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
       <c r="J36" s="34" t="s">
         <v>97</v>
       </c>
@@ -5232,7 +5216,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="90.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="29" t="n">
         <v>107</v>
       </c>
@@ -5248,35 +5232,21 @@
       <c r="E37" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="F37" s="32" t="n">
-        <v>44960</v>
-      </c>
-      <c r="G37" s="42" t="s">
-        <v>160</v>
-      </c>
-      <c r="H37" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="I37" s="42" t="s">
-        <v>162</v>
-      </c>
+      <c r="F37" s="32"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
       <c r="J37" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="M37" s="34" t="s">
         <v>97</v>
       </c>
+      <c r="K37" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
       <c r="N37" s="34"/>
-      <c r="O37" s="34" t="s">
-        <v>54</v>
-      </c>
-      <c r="P37" s="34" t="s">
-        <v>98</v>
-      </c>
+      <c r="O37" s="34"/>
+      <c r="P37" s="34"/>
       <c r="Q37" s="34"/>
       <c r="R37" s="35"/>
       <c r="S37" s="36"/>
@@ -5295,20 +5265,20 @@
         <v>71</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F38" s="32"/>
-      <c r="G38" s="42"/>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
       <c r="J38" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K38" s="34" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L38" s="34"/>
       <c r="M38" s="34"/>
@@ -5333,20 +5303,20 @@
         <v>71</v>
       </c>
       <c r="D39" s="30" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F39" s="32"/>
-      <c r="G39" s="42"/>
-      <c r="H39" s="42"/>
-      <c r="I39" s="42"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
       <c r="J39" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K39" s="34" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="L39" s="34"/>
       <c r="M39" s="34"/>
@@ -5371,20 +5341,20 @@
         <v>71</v>
       </c>
       <c r="D40" s="30" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F40" s="32"/>
-      <c r="G40" s="42"/>
-      <c r="H40" s="42"/>
-      <c r="I40" s="42"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
       <c r="J40" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="L40" s="34"/>
       <c r="M40" s="34"/>
@@ -5409,15 +5379,15 @@
         <v>71</v>
       </c>
       <c r="D41" s="30" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F41" s="32"/>
-      <c r="G41" s="42"/>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
       <c r="J41" s="34" t="s">
         <v>97</v>
       </c>
@@ -5447,15 +5417,15 @@
         <v>71</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F42" s="32"/>
-      <c r="G42" s="42"/>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
       <c r="J42" s="34" t="s">
         <v>97</v>
       </c>
@@ -5485,15 +5455,15 @@
         <v>71</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F43" s="32"/>
-      <c r="G43" s="42"/>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
       <c r="J43" s="34" t="s">
         <v>97</v>
       </c>
@@ -5523,20 +5493,20 @@
         <v>71</v>
       </c>
       <c r="D44" s="30" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F44" s="32"/>
-      <c r="G44" s="42"/>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
       <c r="J44" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L44" s="34"/>
       <c r="M44" s="34"/>
@@ -5561,20 +5531,20 @@
         <v>71</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F45" s="32"/>
-      <c r="G45" s="42"/>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
       <c r="J45" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K45" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L45" s="34"/>
       <c r="M45" s="34"/>
@@ -5599,20 +5569,20 @@
         <v>71</v>
       </c>
       <c r="D46" s="30" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F46" s="32"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
       <c r="J46" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K46" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L46" s="34"/>
       <c r="M46" s="34"/>
@@ -5626,7 +5596,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="29" t="n">
         <v>117</v>
       </c>
@@ -5637,22 +5607,22 @@
         <v>71</v>
       </c>
       <c r="D47" s="30" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F47" s="32" t="n">
         <v>44960</v>
       </c>
-      <c r="G47" s="42" t="s">
+      <c r="G47" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="H47" s="43" t="s">
+        <v>185</v>
+      </c>
+      <c r="I47" s="43" t="s">
         <v>186</v>
-      </c>
-      <c r="H47" s="42" t="s">
-        <v>187</v>
-      </c>
-      <c r="I47" s="42" t="s">
-        <v>188</v>
       </c>
       <c r="J47" s="34" t="s">
         <v>54</v>
@@ -5668,7 +5638,7 @@
       <c r="O47" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P47" s="34" t="s">
+      <c r="P47" s="41" t="s">
         <v>98</v>
       </c>
       <c r="Q47" s="34"/>
@@ -5678,7 +5648,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="29" t="n">
         <v>118</v>
       </c>
@@ -5689,22 +5659,22 @@
         <v>71</v>
       </c>
       <c r="D48" s="30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F48" s="32" t="n">
         <v>44963</v>
       </c>
-      <c r="G48" s="42" t="s">
+      <c r="G48" s="43" t="s">
+        <v>189</v>
+      </c>
+      <c r="H48" s="43" t="s">
+        <v>190</v>
+      </c>
+      <c r="I48" s="43" t="s">
         <v>191</v>
-      </c>
-      <c r="H48" s="42" t="s">
-        <v>192</v>
-      </c>
-      <c r="I48" s="42" t="s">
-        <v>193</v>
       </c>
       <c r="J48" s="34" t="s">
         <v>54</v>
@@ -5720,7 +5690,7 @@
       <c r="O48" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P48" s="34" t="s">
+      <c r="P48" s="41" t="s">
         <v>98</v>
       </c>
       <c r="Q48" s="34"/>
@@ -5741,20 +5711,20 @@
         <v>71</v>
       </c>
       <c r="D49" s="30" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E49" s="31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F49" s="32"/>
-      <c r="G49" s="42"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="43"/>
+      <c r="I49" s="43"/>
       <c r="J49" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K49" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L49" s="34"/>
       <c r="M49" s="34"/>
@@ -5779,20 +5749,20 @@
         <v>71</v>
       </c>
       <c r="D50" s="30" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E50" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F50" s="32"/>
-      <c r="G50" s="42"/>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="43"/>
+      <c r="I50" s="43"/>
       <c r="J50" s="34" t="s">
         <v>97</v>
       </c>
       <c r="K50" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L50" s="34"/>
       <c r="M50" s="34"/>
@@ -5806,7 +5776,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="29" t="n">
         <v>121</v>
       </c>
@@ -5817,22 +5787,22 @@
         <v>71</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E51" s="31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F51" s="32" t="n">
         <v>44971</v>
       </c>
-      <c r="G51" s="42" t="s">
+      <c r="G51" s="43" t="s">
+        <v>198</v>
+      </c>
+      <c r="H51" s="43" t="s">
+        <v>199</v>
+      </c>
+      <c r="I51" s="43" t="s">
         <v>200</v>
-      </c>
-      <c r="H51" s="42" t="s">
-        <v>201</v>
-      </c>
-      <c r="I51" s="42" t="s">
-        <v>202</v>
       </c>
       <c r="J51" s="34" t="s">
         <v>54</v>
@@ -5848,7 +5818,7 @@
       <c r="O51" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="P51" s="34" t="s">
+      <c r="P51" s="41" t="s">
         <v>98</v>
       </c>
       <c r="Q51" s="34"/>
@@ -12603,10 +12573,10 @@
   </sheetPr>
   <dimension ref="A1:D997"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="F10:I10 B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12628,52 +12598,52 @@
         <v>28</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C2" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="D2" s="44" t="s">
         <v>206</v>
-      </c>
-      <c r="C2" s="43" t="s">
-        <v>207</v>
-      </c>
-      <c r="D2" s="43" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>209</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C3" s="43" t="s">
-        <v>210</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" s="45" t="s">
         <v>212</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C4" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12681,13 +12651,13 @@
         <v>48</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C5" s="43" t="s">
-        <v>215</v>
-      </c>
-      <c r="D5" s="43" t="s">
-        <v>216</v>
+        <v>204</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12695,111 +12665,111 @@
         <v>71</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C6" s="43" t="s">
-        <v>217</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>218</v>
+        <v>204</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="45" t="s">
         <v>219</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>220</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>222</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>223</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="45" t="s">
         <v>225</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" s="43" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C10" s="43" t="n">
+        <v>204</v>
+      </c>
+      <c r="C10" s="44" t="n">
         <v>191</v>
       </c>
-      <c r="D10" s="43" t="s">
-        <v>229</v>
+      <c r="D10" s="44" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C11" s="43" t="n">
+        <v>228</v>
+      </c>
+      <c r="C11" s="44" t="n">
         <v>192</v>
       </c>
-      <c r="D11" s="43" t="s">
-        <v>231</v>
+      <c r="D11" s="44" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B12" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C12" s="44" t="n">
+        <v>208</v>
+      </c>
+      <c r="D12" s="44" t="s">
         <v>230</v>
-      </c>
-      <c r="C12" s="43" t="n">
-        <v>208</v>
-      </c>
-      <c r="D12" s="43" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C13" s="43" t="n">
+        <v>228</v>
+      </c>
+      <c r="C13" s="44" t="n">
         <v>224</v>
       </c>
-      <c r="D13" s="44" t="s">
-        <v>233</v>
+      <c r="D13" s="45" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12807,13 +12777,13 @@
         <v>48</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C14" s="43" t="n">
+        <v>228</v>
+      </c>
+      <c r="C14" s="44" t="n">
         <v>240</v>
       </c>
-      <c r="D14" s="43" t="s">
-        <v>234</v>
+      <c r="D14" s="44" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12821,97 +12791,97 @@
         <v>71</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C15" s="43" t="n">
+        <v>228</v>
+      </c>
+      <c r="C15" s="44" t="n">
         <v>256</v>
       </c>
-      <c r="D15" s="44" t="s">
-        <v>235</v>
+      <c r="D15" s="45" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C16" s="43" t="n">
+        <v>228</v>
+      </c>
+      <c r="C16" s="44" t="n">
         <v>272</v>
       </c>
-      <c r="D16" s="44" t="s">
-        <v>236</v>
+      <c r="D16" s="45" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C17" s="43" t="n">
+        <v>228</v>
+      </c>
+      <c r="C17" s="44" t="n">
         <v>288</v>
       </c>
-      <c r="D17" s="44" t="s">
-        <v>237</v>
+      <c r="D17" s="45" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="C18" s="43" t="n">
+        <v>228</v>
+      </c>
+      <c r="C18" s="44" t="n">
         <v>304</v>
       </c>
-      <c r="D18" s="44" t="s">
-        <v>238</v>
+      <c r="D18" s="45" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C19" s="43" t="n">
+        <v>237</v>
+      </c>
+      <c r="C19" s="44" t="n">
         <v>193</v>
       </c>
-      <c r="D19" s="43" t="s">
-        <v>240</v>
+      <c r="D19" s="44" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C20" s="44" t="n">
         <v>209</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="D20" s="44" t="s">
         <v>239</v>
-      </c>
-      <c r="C20" s="43" t="n">
-        <v>209</v>
-      </c>
-      <c r="D20" s="43" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C21" s="43" t="n">
+        <v>237</v>
+      </c>
+      <c r="C21" s="44" t="n">
         <v>225</v>
       </c>
-      <c r="D21" s="44" t="s">
-        <v>242</v>
+      <c r="D21" s="45" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12919,13 +12889,13 @@
         <v>48</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C22" s="43" t="n">
+        <v>237</v>
+      </c>
+      <c r="C22" s="44" t="n">
         <v>241</v>
       </c>
-      <c r="D22" s="43" t="s">
-        <v>243</v>
+      <c r="D22" s="44" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12933,97 +12903,97 @@
         <v>71</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C23" s="43" t="n">
+        <v>237</v>
+      </c>
+      <c r="C23" s="44" t="n">
         <v>257</v>
       </c>
-      <c r="D23" s="44" t="s">
-        <v>244</v>
+      <c r="D23" s="45" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C24" s="43" t="n">
+        <v>237</v>
+      </c>
+      <c r="C24" s="44" t="n">
         <v>273</v>
       </c>
-      <c r="D24" s="44" t="s">
-        <v>245</v>
+      <c r="D24" s="45" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C25" s="43" t="n">
+        <v>237</v>
+      </c>
+      <c r="C25" s="44" t="n">
         <v>289</v>
       </c>
-      <c r="D25" s="44" t="s">
-        <v>246</v>
+      <c r="D25" s="45" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="C26" s="43" t="n">
+        <v>237</v>
+      </c>
+      <c r="C26" s="44" t="n">
         <v>305</v>
       </c>
-      <c r="D26" s="44" t="s">
-        <v>247</v>
+      <c r="D26" s="45" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C27" s="43" t="n">
+        <v>246</v>
+      </c>
+      <c r="C27" s="44" t="n">
         <v>194</v>
       </c>
-      <c r="D27" s="43" t="s">
-        <v>249</v>
+      <c r="D27" s="44" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B28" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="C28" s="44" t="n">
+        <v>210</v>
+      </c>
+      <c r="D28" s="44" t="s">
         <v>248</v>
-      </c>
-      <c r="C28" s="43" t="n">
-        <v>210</v>
-      </c>
-      <c r="D28" s="43" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C29" s="43" t="n">
+        <v>246</v>
+      </c>
+      <c r="C29" s="44" t="n">
         <v>226</v>
       </c>
-      <c r="D29" s="45" t="s">
-        <v>251</v>
+      <c r="D29" s="46" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13031,13 +13001,13 @@
         <v>48</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C30" s="43" t="n">
+        <v>246</v>
+      </c>
+      <c r="C30" s="44" t="n">
         <v>242</v>
       </c>
-      <c r="D30" s="43" t="s">
-        <v>252</v>
+      <c r="D30" s="44" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13045,96 +13015,96 @@
         <v>71</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C31" s="43" t="n">
+        <v>246</v>
+      </c>
+      <c r="C31" s="44" t="n">
         <v>258</v>
       </c>
-      <c r="D31" s="44" t="s">
-        <v>253</v>
+      <c r="D31" s="45" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C32" s="43" t="n">
+        <v>246</v>
+      </c>
+      <c r="C32" s="44" t="n">
         <v>274</v>
       </c>
-      <c r="D32" s="44" t="s">
-        <v>254</v>
+      <c r="D32" s="45" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C33" s="43" t="n">
+        <v>246</v>
+      </c>
+      <c r="C33" s="44" t="n">
         <v>290</v>
       </c>
-      <c r="D33" s="44" t="s">
-        <v>255</v>
+      <c r="D33" s="45" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="C34" s="43" t="n">
+        <v>246</v>
+      </c>
+      <c r="C34" s="44" t="n">
         <v>306</v>
       </c>
-      <c r="D34" s="44" t="s">
-        <v>256</v>
+      <c r="D34" s="45" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C35" s="43" t="n">
+        <v>255</v>
+      </c>
+      <c r="C35" s="44" t="n">
         <v>195</v>
       </c>
-      <c r="D35" s="43" t="n">
+      <c r="D35" s="44" t="n">
         <v>204</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C36" s="43" t="n">
+        <v>255</v>
+      </c>
+      <c r="C36" s="44" t="n">
         <v>211</v>
       </c>
-      <c r="D36" s="43" t="n">
+      <c r="D36" s="44" t="n">
         <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C37" s="43" t="n">
+        <v>255</v>
+      </c>
+      <c r="C37" s="44" t="n">
         <v>227</v>
       </c>
-      <c r="D37" s="44" t="n">
+      <c r="D37" s="45" t="n">
         <v>236</v>
       </c>
     </row>
@@ -13143,12 +13113,12 @@
         <v>48</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C38" s="43" t="n">
+        <v>255</v>
+      </c>
+      <c r="C38" s="44" t="n">
         <v>243</v>
       </c>
-      <c r="D38" s="43" t="n">
+      <c r="D38" s="44" t="n">
         <v>252</v>
       </c>
     </row>
@@ -13157,96 +13127,96 @@
         <v>71</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C39" s="43" t="n">
+        <v>255</v>
+      </c>
+      <c r="C39" s="44" t="n">
         <v>259</v>
       </c>
-      <c r="D39" s="44" t="n">
+      <c r="D39" s="45" t="n">
         <v>268</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C40" s="43" t="n">
+        <v>255</v>
+      </c>
+      <c r="C40" s="44" t="n">
         <v>275</v>
       </c>
-      <c r="D40" s="44" t="n">
+      <c r="D40" s="45" t="n">
         <v>284</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C41" s="43" t="n">
+        <v>255</v>
+      </c>
+      <c r="C41" s="44" t="n">
         <v>291</v>
       </c>
-      <c r="D41" s="44" t="n">
+      <c r="D41" s="45" t="n">
         <v>300</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="C42" s="43" t="n">
+        <v>255</v>
+      </c>
+      <c r="C42" s="44" t="n">
         <v>307</v>
       </c>
-      <c r="D42" s="44" t="n">
+      <c r="D42" s="45" t="n">
         <v>316</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C43" s="43" t="n">
+        <v>256</v>
+      </c>
+      <c r="C43" s="44" t="n">
         <v>196</v>
       </c>
-      <c r="D43" s="43" t="n">
+      <c r="D43" s="44" t="n">
         <v>207</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C44" s="43" t="n">
+        <v>256</v>
+      </c>
+      <c r="C44" s="44" t="n">
         <v>212</v>
       </c>
-      <c r="D44" s="43" t="n">
+      <c r="D44" s="44" t="n">
         <v>223</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C45" s="43" t="n">
+        <v>256</v>
+      </c>
+      <c r="C45" s="44" t="n">
         <v>228</v>
       </c>
-      <c r="D45" s="44" t="n">
+      <c r="D45" s="45" t="n">
         <v>239</v>
       </c>
     </row>
@@ -13255,12 +13225,12 @@
         <v>48</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C46" s="43" t="n">
+        <v>256</v>
+      </c>
+      <c r="C46" s="44" t="n">
         <v>244</v>
       </c>
-      <c r="D46" s="43" t="n">
+      <c r="D46" s="44" t="n">
         <v>255</v>
       </c>
     </row>
@@ -13269,54 +13239,54 @@
         <v>71</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C47" s="43" t="n">
+        <v>256</v>
+      </c>
+      <c r="C47" s="44" t="n">
         <v>260</v>
       </c>
-      <c r="D47" s="44" t="n">
+      <c r="D47" s="45" t="n">
         <v>271</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C48" s="43" t="n">
+        <v>256</v>
+      </c>
+      <c r="C48" s="44" t="n">
         <v>276</v>
       </c>
-      <c r="D48" s="44" t="n">
+      <c r="D48" s="45" t="n">
         <v>287</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="13" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C49" s="43" t="n">
+        <v>256</v>
+      </c>
+      <c r="C49" s="44" t="n">
         <v>292</v>
       </c>
-      <c r="D49" s="44" t="n">
+      <c r="D49" s="45" t="n">
         <v>303</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="C50" s="43" t="n">
+        <v>256</v>
+      </c>
+      <c r="C50" s="44" t="n">
         <v>308</v>
       </c>
-      <c r="D50" s="44" t="n">
+      <c r="D50" s="45" t="n">
         <v>319</v>
       </c>
     </row>
@@ -14285,8 +14255,8 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F10:I10 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14297,26 +14267,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="47" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="46" t="s">
-        <v>259</v>
-      </c>
-      <c r="B2" s="46" t="s">
+      <c r="A2" s="47" t="s">
+        <v>257</v>
+      </c>
+      <c r="B2" s="47" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="46" t="s">
-        <v>260</v>
-      </c>
-      <c r="B3" s="46" t="s">
+      <c r="A3" s="47" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" s="47" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>